<commit_message>
Minor tweaks to auto-annotated NER eval.
</commit_message>
<xml_diff>
--- a/text/eval-annot-raymond.xlsx
+++ b/text/eval-annot-raymond.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="24800" windowHeight="15900" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="22900" windowHeight="15900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
     <sheet name="V2" sheetId="2" r:id="rId2"/>
     <sheet name="Performance" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t># relations (Shows, IsSituatedIn, BelongsTo)</t>
   </si>
@@ -114,6 +114,30 @@
   <si>
     <t>With all documents updated</t>
   </si>
+  <si>
+    <t>Thamme's sol-707 annots NER model</t>
+  </si>
+  <si>
+    <t>Thamme's sol-1159 annots NER model</t>
+  </si>
+  <si>
+    <t>Last 8 docs, v1</t>
+  </si>
+  <si>
+    <t>V2 on the last 8 documents (to compare with Thamme)</t>
+  </si>
+  <si>
+    <t>Thamme's new test set, v1</t>
+  </si>
+  <si>
+    <t>Thamme's new test set, v2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thamme - train </t>
+  </si>
+  <si>
+    <t>Thamme's updated model with all LPSC16 docs</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,11 +206,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -195,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,17 +265,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -238,6 +274,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,42 +576,43 @@
   <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="480" ySplit="3040" activePane="topRight"/>
+      <pane xSplit="480" ySplit="3040" topLeftCell="A45" activePane="bottomRight"/>
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <selection pane="topRight" activeCell="N2" sqref="N2"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62:XFD69"/>
+      <selection pane="bottomRight" activeCell="A62" sqref="A62:A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="13" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="1"/>
@@ -3342,7 +3401,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
+      <c r="A62" s="30">
         <v>2892</v>
       </c>
       <c r="B62" s="7">
@@ -3389,7 +3448,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
+      <c r="A63" s="30">
         <v>2893</v>
       </c>
       <c r="B63" s="7">
@@ -3436,7 +3495,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
+      <c r="A64" s="30">
         <v>2919</v>
       </c>
       <c r="B64" s="7">
@@ -3483,7 +3542,7 @@
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
+      <c r="A65" s="30">
         <v>2940</v>
       </c>
       <c r="B65" s="7">
@@ -3530,7 +3589,7 @@
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
+      <c r="A66" s="30">
         <v>2966</v>
       </c>
       <c r="B66" s="7">
@@ -3577,7 +3636,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="2">
+      <c r="A67" s="30">
         <v>2990</v>
       </c>
       <c r="B67" s="7">
@@ -3624,7 +3683,7 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="2">
+      <c r="A68" s="30">
         <v>3012</v>
       </c>
       <c r="B68" s="7">
@@ -3671,7 +3730,7 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="2">
+      <c r="A69" s="30">
         <v>3021</v>
       </c>
       <c r="B69" s="7">
@@ -3732,36 +3791,36 @@
   <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="480" ySplit="3680" topLeftCell="A5" activePane="bottomRight"/>
+      <pane xSplit="200" ySplit="3700" topLeftCell="A53" activePane="topRight"/>
       <selection activeCell="A3" sqref="A3:XFD3"/>
-      <selection pane="topRight" activeCell="K9" sqref="K9"/>
+      <selection pane="topRight" activeCell="N4" sqref="N4"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" activeCell="C62" sqref="C62:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="13" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="1"/>
@@ -4059,7 +4118,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="18">
+      <c r="A9" s="15">
         <v>1373</v>
       </c>
       <c r="B9" s="7">
@@ -4106,7 +4165,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
+      <c r="A10" s="16">
         <v>1413</v>
       </c>
       <c r="B10" s="7">
@@ -4153,7 +4212,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
+      <c r="A11" s="16">
         <v>1433</v>
       </c>
       <c r="B11" s="7">
@@ -4200,7 +4259,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="19">
+      <c r="A12" s="16">
         <v>1438</v>
       </c>
       <c r="B12" s="7">
@@ -4247,7 +4306,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="19">
+      <c r="A13" s="16">
         <v>1505</v>
       </c>
       <c r="B13" s="7">
@@ -4294,7 +4353,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="18">
+      <c r="A14" s="15">
         <v>1510</v>
       </c>
       <c r="B14" s="7">
@@ -4341,7 +4400,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="19">
+      <c r="A15" s="16">
         <v>1514</v>
       </c>
       <c r="B15" s="7">
@@ -4388,7 +4447,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="19">
+      <c r="A16" s="16">
         <v>1524</v>
       </c>
       <c r="B16" s="7">
@@ -4435,7 +4494,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="19">
+      <c r="A17" s="16">
         <v>1566</v>
       </c>
       <c r="B17" s="7">
@@ -4482,7 +4541,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="19">
+      <c r="A18" s="16">
         <v>1634</v>
       </c>
       <c r="B18" s="7">
@@ -4529,7 +4588,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="19">
+      <c r="A19" s="16">
         <v>1682</v>
       </c>
       <c r="B19" s="7">
@@ -4576,7 +4635,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="19">
+      <c r="A20" s="16">
         <v>1736</v>
       </c>
       <c r="B20" s="7">
@@ -4623,7 +4682,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="19">
+      <c r="A21" s="16">
         <v>1769</v>
       </c>
       <c r="B21" s="7">
@@ -4670,7 +4729,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="19">
+      <c r="A22" s="16">
         <v>1855</v>
       </c>
       <c r="B22" s="7">
@@ -4717,7 +4776,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="19">
+      <c r="A23" s="16">
         <v>1875</v>
       </c>
       <c r="B23" s="7">
@@ -4764,7 +4823,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="19">
+      <c r="A24" s="16">
         <v>1901</v>
       </c>
       <c r="B24" s="7">
@@ -4811,7 +4870,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="19">
+      <c r="A25" s="16">
         <v>1903</v>
       </c>
       <c r="B25" s="7">
@@ -4858,7 +4917,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="19">
+      <c r="A26" s="16">
         <v>1943</v>
       </c>
       <c r="B26" s="7">
@@ -4905,7 +4964,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="18">
+      <c r="A27" s="15">
         <v>1989</v>
       </c>
       <c r="B27" s="7">
@@ -6550,7 +6609,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
+      <c r="A62" s="20">
         <v>2892</v>
       </c>
       <c r="B62" s="7">
@@ -6597,7 +6656,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
+      <c r="A63" s="20">
         <v>2893</v>
       </c>
       <c r="B63" s="7">
@@ -6644,7 +6703,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
+      <c r="A64" s="20">
         <v>2919</v>
       </c>
       <c r="B64" s="7">
@@ -6691,7 +6750,7 @@
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
+      <c r="A65" s="20">
         <v>2940</v>
       </c>
       <c r="B65" s="7">
@@ -6738,7 +6797,7 @@
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
+      <c r="A66" s="20">
         <v>2966</v>
       </c>
       <c r="B66" s="7">
@@ -6785,7 +6844,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="2">
+      <c r="A67" s="20">
         <v>2990</v>
       </c>
       <c r="B67" s="7">
@@ -6832,7 +6891,7 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="2">
+      <c r="A68" s="20">
         <v>3012</v>
       </c>
       <c r="B68" s="7">
@@ -6879,7 +6938,7 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="2">
+      <c r="A69" s="20">
         <v>3021</v>
       </c>
       <c r="B69" s="7">
@@ -6937,461 +6996,657 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" style="20" customWidth="1"/>
-    <col min="14" max="14" width="31" style="20" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="25"/>
+    <col min="7" max="7" width="10.83203125" style="25"/>
+    <col min="10" max="10" width="10.83203125" style="25"/>
+    <col min="13" max="13" width="10.83203125" style="25"/>
+    <col min="14" max="14" width="31" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="20" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="14">
         <f>'V1'!B2</f>
         <v>0.95695695695695693</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="14">
         <f>'V1'!B4</f>
         <v>0.53557422969187674</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="23">
         <f>2*(B3*C3)/(B3+C3)</f>
         <v>0.68678160919540221</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="14">
         <f>'V1'!F2</f>
         <v>0.69158878504672894</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="14">
         <f>'V1'!F4</f>
         <v>0.82913165266106448</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="23">
         <f>2*(E3*F3)/(E3+F3)</f>
         <v>0.75414012738853498</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="14">
         <f>'V1'!J2</f>
         <v>0.48316831683168315</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="14">
         <f>'V1'!J4</f>
         <v>0.89377289377289382</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="23">
         <f>2*(H3*I3)/(H3+I3)</f>
         <v>0.62724935732647813</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="18">
         <f>'V1'!N2</f>
         <v>0.77432712215320909</v>
       </c>
-      <c r="L3" s="21">
+      <c r="L3" s="18">
         <f>'V1'!N4</f>
         <v>0.61946169772256732</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="24">
         <f>2*(K3*L3)/(K3+L3)</f>
         <v>0.68829077524729698</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>0.91300000000000003</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="14">
         <v>0.65500000000000003</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="23">
         <f>2*(B4*C4)/(B4+C4)</f>
         <v>0.76277423469387762</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="23"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="14">
         <v>0.90800000000000003</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="14">
         <v>0.71899999999999997</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="23">
         <f>2*(B5*C5)/(B5+C5)</f>
         <v>0.80252243392747391</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="14">
         <v>0.749</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="14">
         <v>0.76500000000000001</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="23">
         <f>2*(K5*L5)/(K5+L5)</f>
         <v>0.75691545574636721</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>0.90800000000000003</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="14">
         <v>0.71899999999999997</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="23">
         <f>2*(B6*C6)/(B6+C6)</f>
         <v>0.80252243392747391</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="14">
         <v>0.749</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="14">
         <v>0.76400000000000001</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="23">
         <f>2*(K6*L6)/(K6+L6)</f>
         <v>0.75642564441506943</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="14">
         <v>0.82</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <v>0.69</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="23">
         <f>2*(E7*F7)/(E7+F7)</f>
         <v>0.74940397350993382</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17">
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="14">
         <v>0.77700000000000002</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="14">
         <v>0.73399999999999999</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="23">
         <f>2*(K7*L7)/(K7+L7)</f>
         <v>0.75488815354070149</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="14">
         <v>0.70799999999999996</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="14">
         <v>0.81</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="23">
         <f>2*(H8*I8)/(H8+I8)</f>
         <v>0.75557312252964426</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="14">
         <v>0.83599999999999997</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="14">
         <v>0.73</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="23">
         <f>2*(K8*L8)/(K8+L8)</f>
         <v>0.7794125159642401</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="23"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="14">
         <v>0.89200000000000002</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="14">
         <v>0.86199999999999999</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="23">
         <f>2*(B10*C10)/(B10+C10)</f>
         <v>0.87674344355758271</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>0.93100000000000005</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <v>0.67200000000000004</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="23">
         <f>2*(E10*F10)/(E10+F10)</f>
         <v>0.7805764192139738</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="14">
         <v>0.77100000000000002</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="14">
         <v>0.73399999999999999</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="23">
         <f>2*(H10*I10)/(H10+I10)</f>
         <v>0.75204518272425258</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="18">
         <v>0.86899999999999999</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="18">
         <v>0.77900000000000003</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="24">
         <f>2*(K10*L10)/(K10+L10)</f>
         <v>0.8215424757281552</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="A12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="18">
+        <f>1-SUM('V1'!E62:'V1'!E69)/SUM('V1'!C62:'V1'!C69)</f>
+        <v>0.96842105263157896</v>
+      </c>
+      <c r="C12" s="14">
+        <f>(SUM('V1'!B62:'V1'!B69)-SUM('V1'!D62:'V1'!D69))/SUM('V1'!B62:'V1'!B69)</f>
+        <v>0.5679012345679012</v>
+      </c>
+      <c r="D12" s="23">
+        <f>2*(B12*C12)/(B12+C12)</f>
+        <v>0.71595330739299601</v>
+      </c>
+      <c r="E12" s="14">
+        <f>1-SUM('V1'!I62:'V1'!I69)/SUM('V1'!G62:'V1'!G69)</f>
+        <v>0.90384615384615385</v>
+      </c>
+      <c r="F12" s="14">
+        <f>(SUM('V1'!F62:'V1'!F69)-SUM('V1'!H62:'V1'!H69))/SUM('V1'!F62:'V1'!F69)</f>
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="G12" s="24">
+        <f>2*(E12*F12)/(E12+F12)</f>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="H12" s="14">
+        <f>1-SUM('V1'!M62:'V1'!M69)/SUM('V1'!K62:'V1'!K69)</f>
+        <v>0.85185185185185186</v>
+      </c>
+      <c r="I12" s="14">
+        <f>(SUM('V1'!J62:'V1'!J69)-SUM('V1'!L62:'V1'!L69))/SUM('V1'!J62:'V1'!J69)</f>
+        <v>0.85185185185185186</v>
+      </c>
+      <c r="J12" s="23">
+        <f>2*(H12*I12)/(H12+I12)</f>
+        <v>0.85185185185185186</v>
+      </c>
+      <c r="K12" s="18">
+        <f>1-(SUM('V1'!E62:'V1'!E69)+SUM('V1'!I62:'V1'!I69)+SUM('V1'!M62:'V1'!M69))/(SUM('V1'!C62:'V1'!C69)+SUM('V1'!G62:'V1'!G69)+SUM('V1'!K62:'V1'!K69))</f>
+        <v>0.93103448275862066</v>
+      </c>
+      <c r="L12" s="14">
+        <f>(SUM('V1'!B62:'V1'!B69)-SUM('V1'!D62:'V1'!D69)+SUM('V1'!F62:'V1'!F69)-SUM('V1'!H62:'V1'!H69)+SUM('V1'!J62:'V1'!J69)-SUM('V1'!L62:'V1'!L69))/(SUM('V1'!B62:'V1'!B69)+SUM('V1'!F62:'V1'!F69)+SUM('V1'!J62:'V1'!J69))</f>
+        <v>0.68354430379746833</v>
+      </c>
+      <c r="M12" s="26">
+        <f>2*(K12*L12)/(K12+L12)</f>
+        <v>0.7883211678832116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="14">
+        <f>1-SUM('V2'!E62:'V2'!E69)/SUM('V2'!C62:'V2'!C69)</f>
+        <v>0.88421052631578945</v>
+      </c>
+      <c r="C13" s="18">
+        <f>(SUM('V2'!B62:'V2'!B69)-SUM('V2'!D62:'V2'!D69))/SUM('V2'!B62:'V2'!B69)</f>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="D13" s="24">
+        <f>2*(B13*C13)/(B13+C13)</f>
+        <v>0.85279187817258884</v>
+      </c>
+      <c r="E13" s="18">
+        <f>1-SUM('V2'!I62:'V2'!I69)/SUM('V2'!G62:'V2'!G69)</f>
+        <v>0.98076923076923073</v>
+      </c>
+      <c r="F13" s="14">
+        <f>(SUM('V2'!F62:'V2'!F69)-SUM('V2'!H62:'V2'!H69))/SUM('V2'!F62:'V2'!F69)</f>
+        <v>0.68</v>
+      </c>
+      <c r="G13" s="23">
+        <f>2*(E13*F13)/(E13+F13)</f>
+        <v>0.80314960629921262</v>
+      </c>
+      <c r="H13" s="18">
+        <f>1-SUM('V2'!M62:'V2'!M69)/SUM('V2'!K62:'V2'!K69)</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="14">
+        <f>(SUM('V2'!J62:'V2'!J69)-SUM('V2'!L62:'V2'!L69))/SUM('V2'!J62:'V2'!J69)</f>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="J13" s="24">
+        <f>2*(H13*I13)/(H13+I13)</f>
+        <v>0.9</v>
+      </c>
+      <c r="K13" s="18">
+        <f>1-(SUM('V2'!E62:'V2'!E69)+SUM('V2'!I62:'V2'!I69)+SUM('V2'!M62:'V2'!M69))/(SUM('V2'!C62:'V2'!C69)+SUM('V2'!G62:'V2'!G69)+SUM('V2'!K62:'V2'!K69))</f>
+        <v>0.93103448275862066</v>
+      </c>
+      <c r="L13" s="18">
+        <f>(SUM('V2'!B62:'V2'!B69)-SUM('V2'!D62:'V2'!D69)+SUM('V2'!F62:'V2'!F69)-SUM('V2'!H62:'V2'!H69)+SUM('V2'!J62:'V2'!J69)-SUM('V2'!L62:'V2'!L69))/(SUM('V2'!B62:'V2'!B69)+SUM('V2'!F62:'V2'!F69)+SUM('V2'!J62:'V2'!J69))</f>
+        <v>0.77142857142857146</v>
+      </c>
+      <c r="M13" s="24">
+        <f>2*(K13*L13)/(K13+L13)</f>
+        <v>0.84375000000000011</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="A14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.63060000000000005</v>
+      </c>
+      <c r="D14" s="23">
+        <f>2*(B14*C14)/(B14+C14)</f>
+        <v>0.6965076398750355</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.68630000000000002</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.85370000000000001</v>
+      </c>
+      <c r="G14" s="23">
+        <f>2*(E14*F14)/(E14+F14)</f>
+        <v>0.76090170129870127</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0.60870000000000002</v>
+      </c>
+      <c r="I14" s="18">
+        <v>1</v>
+      </c>
+      <c r="J14" s="23">
+        <f>2*(H14*I14)/(H14+I14)</f>
+        <v>0.75676011686454903</v>
+      </c>
+      <c r="K14" s="14">
+        <v>0.68</v>
+      </c>
+      <c r="L14" s="14">
+        <v>0.71689999999999998</v>
+      </c>
+      <c r="M14" s="23">
+        <f>2*(K14*L14)/(K14+L14)</f>
+        <v>0.69796263154127003</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
+      <c r="A15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="D15" s="23">
+        <f>2*(B15*C15)/(B15+C15)</f>
+        <v>0.76922485138278629</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1</v>
+      </c>
+      <c r="G15" s="23">
+        <f>2*(E15*F15)/(E15+F15)</f>
+        <v>0.49996249906247658</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0.56520000000000004</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0.65</v>
+      </c>
+      <c r="J15" s="23">
+        <f>2*(H15*I15)/(H15+I15)</f>
+        <v>0.604641211323239</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0.73429999999999995</v>
+      </c>
+      <c r="M15" s="23">
+        <f>2*(K15*L15)/(K15+L15)</f>
+        <v>0.66039121636813314</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
+      <c r="A16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.67230000000000001</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0.76559999999999995</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.84309999999999996</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.91490000000000005</v>
+      </c>
+      <c r="G16" s="23">
+        <v>0.87760000000000005</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0.95450000000000002</v>
+      </c>
+      <c r="J16" s="23">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="K16" s="14">
+        <v>0.86709999999999998</v>
+      </c>
+      <c r="L16" s="14">
+        <v>0.75390000000000001</v>
+      </c>
+      <c r="M16" s="23">
+        <v>0.80220000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="23"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="23"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="23"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Added separate evaluation for dev and test sets in LPSC 2016.
</commit_message>
<xml_diff>
--- a/text/eval-annot-raymond.xlsx
+++ b/text/eval-annot-raymond.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="460" windowWidth="18960" windowHeight="15900" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-920" yWindow="2200" windowWidth="22080" windowHeight="15900" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LPSC15-V1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="39">
   <si>
     <t># relations (Shows, IsSituatedIn, BelongsTo)</t>
   </si>
@@ -144,6 +144,12 @@
   <si>
     <t>F1</t>
   </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
 </sst>
 </file>
 
@@ -220,7 +226,7 @@
       <name val="Lucida Grande"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +248,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +281,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -322,17 +334,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -633,24 +649,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
@@ -3841,24 +3857,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
@@ -7049,24 +7065,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
@@ -7168,28 +7184,28 @@
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="30">
         <f>2*B3*B4/(B3+B4)</f>
         <v>0.88036345280161532</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
-      <c r="F5" s="32">
+      <c r="F5" s="30">
         <f>2*F3*F4/(F3+F4)</f>
         <v>0.70637408568443039</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
-      <c r="J5" s="32">
+      <c r="J5" s="30">
         <f>2*J3*J4/(J3+J4)</f>
         <v>0.75098039215686285</v>
       </c>
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
-      <c r="N5" s="32">
+      <c r="N5" s="30">
         <f>2*N3*N4/(N3+N4)</f>
         <v>0.80482117558109545</v>
       </c>
@@ -7398,7 +7414,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="33">
+      <c r="A10" s="31">
         <v>1373</v>
       </c>
       <c r="B10" s="7">
@@ -7445,7 +7461,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="34">
+      <c r="A11" s="32">
         <v>1413</v>
       </c>
       <c r="B11" s="7">
@@ -7492,7 +7508,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="34">
+      <c r="A12" s="32">
         <v>1433</v>
       </c>
       <c r="B12" s="7">
@@ -7539,7 +7555,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="34">
+      <c r="A13" s="32">
         <v>1438</v>
       </c>
       <c r="B13" s="7">
@@ -7586,7 +7602,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="34">
+      <c r="A14" s="32">
         <v>1505</v>
       </c>
       <c r="B14" s="7">
@@ -7633,7 +7649,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="33">
+      <c r="A15" s="31">
         <v>1510</v>
       </c>
       <c r="B15" s="7">
@@ -7680,7 +7696,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="34">
+      <c r="A16" s="32">
         <v>1514</v>
       </c>
       <c r="B16" s="7">
@@ -7727,7 +7743,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="34">
+      <c r="A17" s="32">
         <v>1524</v>
       </c>
       <c r="B17" s="7">
@@ -7774,7 +7790,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="34">
+      <c r="A18" s="32">
         <v>1566</v>
       </c>
       <c r="B18" s="7">
@@ -7821,7 +7837,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="34">
+      <c r="A19" s="32">
         <v>1634</v>
       </c>
       <c r="B19" s="7">
@@ -7868,7 +7884,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="34">
+      <c r="A20" s="32">
         <v>1682</v>
       </c>
       <c r="B20" s="7">
@@ -7915,7 +7931,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="34">
+      <c r="A21" s="32">
         <v>1736</v>
       </c>
       <c r="B21" s="7">
@@ -7962,7 +7978,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="34">
+      <c r="A22" s="32">
         <v>1769</v>
       </c>
       <c r="B22" s="7">
@@ -8009,7 +8025,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="34">
+      <c r="A23" s="32">
         <v>1875</v>
       </c>
       <c r="B23" s="7">
@@ -8056,7 +8072,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="34">
+      <c r="A24" s="32">
         <v>1901</v>
       </c>
       <c r="B24" s="7">
@@ -8103,7 +8119,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="34">
+      <c r="A25" s="32">
         <v>1903</v>
       </c>
       <c r="B25" s="7">
@@ -8150,7 +8166,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="34">
+      <c r="A26" s="32">
         <v>1943</v>
       </c>
       <c r="B26" s="7">
@@ -8197,7 +8213,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="33">
+      <c r="A27" s="31">
         <v>1989</v>
       </c>
       <c r="B27" s="7">
@@ -9842,7 +9858,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="33">
+      <c r="A62" s="31">
         <v>2892</v>
       </c>
       <c r="B62" s="7">
@@ -9889,7 +9905,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="33">
+      <c r="A63" s="31">
         <v>2893</v>
       </c>
       <c r="B63" s="7">
@@ -9936,7 +9952,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" s="33">
+      <c r="A64" s="31">
         <v>2919</v>
       </c>
       <c r="B64" s="7">
@@ -9983,7 +9999,7 @@
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="33">
+      <c r="A65" s="31">
         <v>2940</v>
       </c>
       <c r="B65" s="7">
@@ -10030,7 +10046,7 @@
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="33">
+      <c r="A66" s="31">
         <v>2966</v>
       </c>
       <c r="B66" s="7">
@@ -10077,7 +10093,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="33">
+      <c r="A67" s="31">
         <v>2990</v>
       </c>
       <c r="B67" s="7">
@@ -10124,7 +10140,7 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="33">
+      <c r="A68" s="31">
         <v>3012</v>
       </c>
       <c r="B68" s="7">
@@ -10171,7 +10187,7 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="33">
+      <c r="A69" s="31">
         <v>3021</v>
       </c>
       <c r="B69" s="7">
@@ -10243,24 +10259,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
@@ -10362,28 +10378,28 @@
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="30">
         <f>2*B3*B4/(B3+B4)</f>
         <v>0.79616963064295476</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
-      <c r="F5" s="32">
+      <c r="F5" s="30">
         <f>2*F3*F4/(F3+F4)</f>
         <v>0.8015873015873014</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
-      <c r="J5" s="32">
+      <c r="J5" s="30">
         <f>2*J3*J4/(J3+J4)</f>
         <v>0.75023386342376042</v>
       </c>
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
-      <c r="N5" s="32">
+      <c r="N5" s="30">
         <f>2*N3*N4/(N3+N4)</f>
         <v>0.78692298317753628</v>
       </c>
@@ -10584,7 +10600,7 @@
       <c r="O9" s="7"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="33">
+      <c r="A10" s="31">
         <v>1373</v>
       </c>
       <c r="B10" s="7">
@@ -10627,7 +10643,7 @@
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="34">
+      <c r="A11" s="32">
         <v>1413</v>
       </c>
       <c r="B11" s="7">
@@ -10670,7 +10686,7 @@
       <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="34">
+      <c r="A12" s="32">
         <v>1433</v>
       </c>
       <c r="B12" s="7">
@@ -10713,7 +10729,7 @@
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="34">
+      <c r="A13" s="32">
         <v>1438</v>
       </c>
       <c r="B13" s="7">
@@ -10756,7 +10772,7 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="34">
+      <c r="A14" s="32">
         <v>1505</v>
       </c>
       <c r="B14" s="7">
@@ -10799,7 +10815,7 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="33">
+      <c r="A15" s="31">
         <v>1510</v>
       </c>
       <c r="B15" s="7">
@@ -10842,7 +10858,7 @@
       <c r="O15" s="7"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="34">
+      <c r="A16" s="32">
         <v>1514</v>
       </c>
       <c r="B16" s="7">
@@ -10885,7 +10901,7 @@
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="34">
+      <c r="A17" s="32">
         <v>1524</v>
       </c>
       <c r="B17" s="7">
@@ -10928,7 +10944,7 @@
       <c r="O17" s="7"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="34">
+      <c r="A18" s="32">
         <v>1566</v>
       </c>
       <c r="B18" s="7">
@@ -10971,7 +10987,7 @@
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="34">
+      <c r="A19" s="32">
         <v>1634</v>
       </c>
       <c r="B19" s="7">
@@ -11014,7 +11030,7 @@
       <c r="O19" s="7"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="34">
+      <c r="A20" s="32">
         <v>1682</v>
       </c>
       <c r="B20" s="7">
@@ -11057,7 +11073,7 @@
       <c r="O20" s="7"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="34">
+      <c r="A21" s="32">
         <v>1736</v>
       </c>
       <c r="B21" s="7">
@@ -11100,7 +11116,7 @@
       <c r="O21" s="7"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="34">
+      <c r="A22" s="32">
         <v>1769</v>
       </c>
       <c r="B22" s="7">
@@ -11143,7 +11159,7 @@
       <c r="O22" s="7"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="34">
+      <c r="A23" s="32">
         <v>1875</v>
       </c>
       <c r="B23" s="7">
@@ -11186,7 +11202,7 @@
       <c r="O23" s="7"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="34">
+      <c r="A24" s="32">
         <v>1901</v>
       </c>
       <c r="B24" s="7">
@@ -11229,7 +11245,7 @@
       <c r="O24" s="7"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="34">
+      <c r="A25" s="32">
         <v>1903</v>
       </c>
       <c r="B25" s="7">
@@ -11272,7 +11288,7 @@
       <c r="O25" s="7"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="34">
+      <c r="A26" s="32">
         <v>1943</v>
       </c>
       <c r="B26" s="7">
@@ -11315,7 +11331,7 @@
       <c r="O26" s="7"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="33">
+      <c r="A27" s="31">
         <v>1989</v>
       </c>
       <c r="B27" s="7">
@@ -12820,7 +12836,7 @@
       <c r="O61" s="7"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="33">
+      <c r="A62" s="31">
         <v>2892</v>
       </c>
       <c r="B62" s="7">
@@ -12863,7 +12879,7 @@
       <c r="O62" s="7"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="33">
+      <c r="A63" s="31">
         <v>2893</v>
       </c>
       <c r="B63" s="7">
@@ -12906,7 +12922,7 @@
       <c r="O63" s="7"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" s="33">
+      <c r="A64" s="31">
         <v>2919</v>
       </c>
       <c r="B64" s="7">
@@ -12949,7 +12965,7 @@
       <c r="O64" s="7"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="33">
+      <c r="A65" s="31">
         <v>2940</v>
       </c>
       <c r="B65" s="7">
@@ -12992,7 +13008,7 @@
       <c r="O65" s="7"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="33">
+      <c r="A66" s="31">
         <v>2966</v>
       </c>
       <c r="B66" s="7">
@@ -13035,7 +13051,7 @@
       <c r="O66" s="7"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="33">
+      <c r="A67" s="31">
         <v>2990</v>
       </c>
       <c r="B67" s="7">
@@ -13078,7 +13094,7 @@
       <c r="O67" s="7"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="33">
+      <c r="A68" s="31">
         <v>3012</v>
       </c>
       <c r="B68" s="7">
@@ -13121,7 +13137,7 @@
       <c r="O68" s="7"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="33">
+      <c r="A69" s="31">
         <v>3021</v>
       </c>
       <c r="B69" s="7">
@@ -13175,36 +13191,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3060"/>
-      <selection activeCell="N3" sqref="N3"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane ySplit="3060" topLeftCell="A2"/>
+      <selection activeCell="P5" sqref="P5"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="12" t="s">
         <v>14</v>
       </c>
@@ -13218,28 +13234,45 @@
         <f>(B7-D7)/C7</f>
         <v>0.95107398568019097</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="E2" s="27"/>
       <c r="F2" s="8">
         <f>(F7-H7)/G7</f>
         <v>0.9422382671480144</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>38</v>
+      </c>
       <c r="I2" s="27"/>
       <c r="J2" s="8">
         <f>(J7-L7)/K7</f>
         <v>0.74285714285714288</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
+      <c r="K2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>38</v>
+      </c>
       <c r="M2" s="27"/>
       <c r="N2" s="10">
         <f>(B7+F7+J7-D7-H7-L7)/(C7+G7+K7)</f>
         <v>0.90642939150401836</v>
       </c>
-      <c r="O2" s="1"/>
+      <c r="O2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -13249,27 +13282,52 @@
         <f>1-E7/C7</f>
         <v>0.95107398568019097</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="8">
+        <f>1-E8/C8</f>
+        <v>0.93633952254641906</v>
+      </c>
+      <c r="D3" s="8">
+        <f>1-E9/C9</f>
+        <v>0.96312364425162689</v>
+      </c>
       <c r="E3" s="27"/>
       <c r="F3" s="8">
         <f>1-I7/G7</f>
         <v>0.9422382671480144</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="G3" s="8">
+        <f>1-I8/G8</f>
+        <v>0.92561983471074383</v>
+      </c>
+      <c r="H3" s="8">
+        <f>1-I9/G9</f>
+        <v>0.95512820512820518</v>
+      </c>
       <c r="I3" s="27"/>
       <c r="J3" s="8">
         <f>1-M7/K7</f>
         <v>0.74285714285714288</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
+      <c r="K3" s="8">
+        <f>1-M8/K8</f>
+        <v>0.83766233766233766</v>
+      </c>
+      <c r="L3" s="8">
+        <f>1-M9/K9</f>
+        <v>0.66836734693877553</v>
+      </c>
       <c r="M3" s="27"/>
       <c r="N3" s="10">
         <v>0.90600000000000003</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="O3" s="10">
+        <f>(B8+F8+J8-D8-H8-L8)/(C8+G8+K8)</f>
+        <v>0.91332470892626128</v>
+      </c>
+      <c r="P3" s="10">
+        <f>(B9+F9+J9-D9-H9-L9)/(C9+G9+K9)</f>
+        <v>0.90092879256965941</v>
+      </c>
     </row>
     <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -13279,59 +13337,109 @@
         <f>(B7-D7)/B7</f>
         <v>0.89651293588301462</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
+      <c r="C4" s="8">
+        <f>(B8-D8)/B8</f>
+        <v>0.93139841688654357</v>
+      </c>
+      <c r="D4" s="8">
+        <f>(B9-D9)/B9</f>
+        <v>0.87058823529411766</v>
+      </c>
       <c r="E4" s="27"/>
       <c r="F4" s="8">
         <f>(F7-H7)/F7</f>
         <v>0.97570093457943929</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="8">
+        <f>(F8-H8)/F8</f>
+        <v>0.97391304347826091</v>
+      </c>
+      <c r="H4" s="8">
+        <f>(F9-H9)/F9</f>
+        <v>0.9770491803278688</v>
+      </c>
       <c r="I4" s="27"/>
       <c r="J4" s="8">
         <f>(J7-L7)/J7</f>
         <v>0.72625698324022347</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
+      <c r="K4" s="8">
+        <f>(J8-L8)/J8</f>
+        <v>0.82165605095541405</v>
+      </c>
+      <c r="L4" s="8">
+        <f>(J9-L9)/J9</f>
+        <v>0.65174129353233834</v>
+      </c>
       <c r="M4" s="27"/>
       <c r="N4" s="10">
         <f>(B7+F7+J7-D7-H7-L7)/(B7+F7+J7)</f>
         <v>0.88608305274971944</v>
       </c>
-      <c r="O4" s="1"/>
+      <c r="O4" s="10">
+        <f>(B8+F8+J8-D8-H8-L8)/(B8+F8+J8)</f>
+        <v>0.92167101827676245</v>
+      </c>
+      <c r="P4" s="10">
+        <f>(B9+F9+J9-D9-H9-L9)/(B9+F9+J9)</f>
+        <v>0.85925196850393704</v>
+      </c>
     </row>
     <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="30">
         <f>2*B3*B4/(B3+B4)</f>
         <v>0.92298784018529256</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="C5" s="30">
+        <f>2*C3*C4/(C3+C4)</f>
+        <v>0.93386243386243395</v>
+      </c>
+      <c r="D5" s="30">
+        <f>2*D3*D4/(D3+D4)</f>
+        <v>0.91452111225540678</v>
+      </c>
       <c r="E5" s="27"/>
-      <c r="F5" s="32">
+      <c r="F5" s="30">
         <f>2*F3*F4/(F3+F4)</f>
         <v>0.95867768595041325</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="G5" s="30">
+        <f>2*G3*G4/(G3+G4)</f>
+        <v>0.94915254237288138</v>
+      </c>
+      <c r="H5" s="30">
+        <f>2*H3*H4/(H3+H4)</f>
+        <v>0.96596434359805516</v>
+      </c>
       <c r="I5" s="27"/>
-      <c r="J5" s="32">
+      <c r="J5" s="30">
         <f>2*J3*J4/(J3+J4)</f>
         <v>0.7344632768361582</v>
       </c>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
+      <c r="K5" s="30">
+        <f>2*K3*K4/(K3+K4)</f>
+        <v>0.82958199356913187</v>
+      </c>
+      <c r="L5" s="30">
+        <f>2*L3*L4/(L3+L4)</f>
+        <v>0.65994962216624697</v>
+      </c>
       <c r="M5" s="27"/>
-      <c r="N5" s="32">
+      <c r="N5" s="30">
         <f>2*N3*N4/(N3+N4)</f>
         <v>0.89593084936489586</v>
       </c>
-      <c r="O5" s="1"/>
+      <c r="O5" s="30">
+        <f>2*O3*O4/(O3+O4)</f>
+        <v>0.91747888239116304</v>
+      </c>
+      <c r="P5" s="30">
+        <f>2*P3*P4/(P3+P4)</f>
+        <v>0.87959697732997488</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -13385,7 +13493,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B7:O7" si="0">SUM(B8:B70)</f>
+        <f t="shared" ref="B7:O8" si="0">SUM(B10:B72)</f>
         <v>889</v>
       </c>
       <c r="C7" s="3">
@@ -13442,132 +13550,154 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>1029</v>
-      </c>
-      <c r="B8" s="2">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2">
-        <v>15</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="A8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3">
+        <f>SUM(B10:B29)</f>
+        <v>379</v>
+      </c>
+      <c r="C8" s="3">
+        <f>SUM(C10:C29)</f>
+        <v>377</v>
+      </c>
+      <c r="D8" s="3">
+        <f>SUM(D10:D29)</f>
+        <v>26</v>
+      </c>
+      <c r="E8" s="3">
+        <f>SUM(E10:E29)</f>
+        <v>24</v>
+      </c>
+      <c r="F8" s="3">
+        <f>SUM(F10:F29)</f>
+        <v>230</v>
+      </c>
+      <c r="G8" s="3">
+        <f>SUM(G10:G29)</f>
+        <v>242</v>
+      </c>
+      <c r="H8" s="3">
+        <f>SUM(H10:H29)</f>
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <f>SUM(I10:I29)</f>
         <v>18</v>
       </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>3</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="J8" s="3">
+        <f>SUM(J10:J29)</f>
+        <v>157</v>
+      </c>
+      <c r="K8" s="3">
+        <f>SUM(K10:K29)</f>
+        <v>154</v>
+      </c>
+      <c r="L8" s="3">
+        <f>SUM(L10:L29)</f>
+        <v>28</v>
+      </c>
+      <c r="M8" s="3">
+        <f>SUM(M10:M29)</f>
+        <v>25</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>1155</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>15</v>
-      </c>
-      <c r="G9" s="2">
-        <v>24</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
-        <v>10</v>
-      </c>
-      <c r="J9" s="2">
-        <v>39</v>
-      </c>
-      <c r="K9" s="2">
-        <v>40</v>
-      </c>
-      <c r="L9" s="2">
-        <v>6</v>
-      </c>
-      <c r="M9" s="2">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3">
+        <f>SUM(B30:B64)</f>
+        <v>510</v>
+      </c>
+      <c r="C9" s="3">
+        <f>SUM(C30:C64)</f>
+        <v>461</v>
+      </c>
+      <c r="D9" s="3">
+        <f>SUM(D30:D64)</f>
+        <v>66</v>
+      </c>
+      <c r="E9" s="3">
+        <f>SUM(E30:E64)</f>
+        <v>17</v>
+      </c>
+      <c r="F9" s="3">
+        <f>SUM(F30:F64)</f>
+        <v>305</v>
+      </c>
+      <c r="G9" s="3">
+        <f>SUM(G30:G64)</f>
+        <v>312</v>
+      </c>
+      <c r="H9" s="3">
+        <f>SUM(H30:H64)</f>
         <v>7</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="I9" s="3">
+        <f>SUM(I30:I64)</f>
+        <v>14</v>
+      </c>
+      <c r="J9" s="3">
+        <f>SUM(J30:J64)</f>
+        <v>201</v>
+      </c>
+      <c r="K9" s="3">
+        <f>SUM(K30:K64)</f>
+        <v>196</v>
+      </c>
+      <c r="L9" s="3">
+        <f>SUM(L30:L64)</f>
+        <v>70</v>
+      </c>
+      <c r="M9" s="3">
+        <f>SUM(M30:M64)</f>
+        <v>65</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>1163</v>
+        <v>1029</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
       </c>
       <c r="C10" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2">
+        <v>18</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
         <v>3</v>
       </c>
-      <c r="F10" s="2">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2">
-        <v>12</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
       <c r="J10" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -13575,43 +13705,43 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>1206</v>
+        <v>1155</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G11" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H11" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J11" s="2">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="K11" s="2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L11" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M11" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -13619,25 +13749,25 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>1318</v>
+        <v>1163</v>
       </c>
       <c r="B12" s="2">
         <v>10</v>
       </c>
       <c r="C12" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G12" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
@@ -13646,16 +13776,16 @@
         <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K12" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -13663,40 +13793,40 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>1322</v>
+        <v>1206</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
       </c>
       <c r="J13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
@@ -13707,25 +13837,25 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>1336</v>
+        <v>1318</v>
       </c>
       <c r="B14" s="2">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
@@ -13734,10 +13864,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L14" s="2">
         <v>1</v>
@@ -13751,25 +13881,25 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>1347</v>
+        <v>1322</v>
       </c>
       <c r="B15" s="2">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="D15" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
@@ -13778,10 +13908,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <v>1</v>
@@ -13795,25 +13925,25 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>1348</v>
+        <v>1336</v>
       </c>
       <c r="B16" s="2">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
       </c>
       <c r="F16" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G16" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
@@ -13822,16 +13952,16 @@
         <v>0</v>
       </c>
       <c r="J16" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="K16" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -13839,25 +13969,25 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>1364</v>
+        <v>1347</v>
       </c>
       <c r="B17" s="2">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C17" s="2">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G17" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H17" s="2">
         <v>0</v>
@@ -13866,13 +13996,13 @@
         <v>0</v>
       </c>
       <c r="J17" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="K17" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L17" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M17" s="2">
         <v>0</v>
@@ -13883,25 +14013,25 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>1495</v>
+        <v>1348</v>
       </c>
       <c r="B18" s="2">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" s="2">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G18" s="2">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
@@ -13910,16 +14040,16 @@
         <v>0</v>
       </c>
       <c r="J18" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K18" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
       </c>
       <c r="M18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -13927,40 +14057,40 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>1507</v>
+        <v>1364</v>
       </c>
       <c r="B19" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="G19" s="2">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M19" s="2">
         <v>0</v>
@@ -13971,25 +14101,25 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>1536</v>
+        <v>1495</v>
       </c>
       <c r="B20" s="2">
         <v>11</v>
       </c>
       <c r="C20" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2">
         <v>1</v>
       </c>
       <c r="F20" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G20" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
@@ -13998,16 +14128,16 @@
         <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L20" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M20" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -14015,40 +14145,40 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>1604</v>
+        <v>1507</v>
       </c>
       <c r="B21" s="2">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F21" s="2">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="G21" s="2">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
       <c r="I21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K21" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="2">
         <v>0</v>
@@ -14059,43 +14189,43 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>1614</v>
+        <v>1536</v>
       </c>
       <c r="B22" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D22" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G22" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K22" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L22" s="2">
         <v>3</v>
       </c>
       <c r="M22" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -14103,25 +14233,25 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>1675</v>
+        <v>1604</v>
       </c>
       <c r="B23" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G23" s="2">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
@@ -14130,16 +14260,16 @@
         <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="K23" s="2">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="L23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -14147,43 +14277,43 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>1703</v>
+        <v>1614</v>
       </c>
       <c r="B24" s="2">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>7</v>
+      </c>
+      <c r="G24" s="2">
+        <v>6</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>10</v>
+      </c>
+      <c r="K24" s="2">
+        <v>8</v>
+      </c>
+      <c r="L24" s="2">
         <v>3</v>
       </c>
-      <c r="F24" s="2">
-        <v>25</v>
-      </c>
-      <c r="G24" s="2">
-        <v>28</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2">
-        <v>3</v>
-      </c>
-      <c r="J24" s="2">
-        <v>2</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
-      <c r="L24" s="2">
-        <v>1</v>
-      </c>
       <c r="M24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -14191,13 +14321,13 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>1739</v>
+        <v>1675</v>
       </c>
       <c r="B25" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -14206,10 +14336,10 @@
         <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G25" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
@@ -14218,16 +14348,16 @@
         <v>0</v>
       </c>
       <c r="J25" s="2">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="K25" s="2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -14235,40 +14365,40 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>1761</v>
+        <v>1703</v>
       </c>
       <c r="B26" s="2">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="C26" s="2">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
       </c>
       <c r="E26" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F26" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G26" s="2">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="2">
         <v>0</v>
@@ -14279,43 +14409,43 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>1767</v>
+        <v>1739</v>
       </c>
       <c r="B27" s="2">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D27" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
       </c>
       <c r="F27" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G27" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>
       <c r="I27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K27" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -14323,16 +14453,16 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>1770</v>
+        <v>1761</v>
       </c>
       <c r="B28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -14350,13 +14480,13 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
       </c>
       <c r="L28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="2">
         <v>0</v>
@@ -14367,84 +14497,84 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>1826</v>
+        <v>1767</v>
       </c>
       <c r="B29" s="2">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C29" s="2">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E29" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G29" s="2">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K29" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L29" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M29" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>1886</v>
+      <c r="A30" s="36">
+        <v>1770</v>
       </c>
       <c r="B30" s="2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
       </c>
       <c r="I30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K30" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M30" s="2">
         <v>0</v>
@@ -14454,129 +14584,129 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>1899</v>
+      <c r="A31" s="36">
+        <v>1826</v>
       </c>
       <c r="B31" s="2">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" s="2">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G31" s="2">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="2">
         <v>0</v>
       </c>
       <c r="K31" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L31" s="2">
         <v>0</v>
       </c>
       <c r="M31" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>1990</v>
+      <c r="A32" s="36">
+        <v>1886</v>
       </c>
       <c r="B32" s="2">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C32" s="2">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D32" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" s="2">
+        <v>49</v>
+      </c>
+      <c r="G32" s="2">
+        <v>50</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
         <v>9</v>
       </c>
-      <c r="G32" s="2">
-        <v>10</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2">
-        <v>12</v>
-      </c>
       <c r="K32" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="L32" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M32" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <v>2013</v>
+      <c r="A33" s="36">
+        <v>1899</v>
       </c>
       <c r="B33" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E33" s="2">
         <v>0</v>
       </c>
       <c r="F33" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G33" s="2">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>
@@ -14586,70 +14716,70 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>2037</v>
+      <c r="A34" s="36">
+        <v>1990</v>
       </c>
       <c r="B34" s="2">
+        <v>37</v>
+      </c>
+      <c r="C34" s="2">
+        <v>38</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
         <v>9</v>
       </c>
-      <c r="C34" s="2">
-        <v>7</v>
-      </c>
-      <c r="D34" s="2">
-        <v>2</v>
-      </c>
-      <c r="E34" s="2">
-        <v>0</v>
-      </c>
-      <c r="F34" s="2">
-        <v>29</v>
-      </c>
       <c r="G34" s="2">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
       </c>
       <c r="I34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K34" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M34" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>2044</v>
+      <c r="A35" s="36">
+        <v>2013</v>
       </c>
       <c r="B35" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C35" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D35" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
       </c>
       <c r="F35" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G35" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
@@ -14658,57 +14788,57 @@
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K35" s="2">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="L35" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M35" s="2">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>2046</v>
+      <c r="A36" s="36">
+        <v>2037</v>
       </c>
       <c r="B36" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D36" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
       </c>
       <c r="F36" s="2">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="G36" s="2">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
       </c>
       <c r="I36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K36" s="2">
         <v>0</v>
       </c>
       <c r="L36" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
         <v>0</v>
@@ -14718,71 +14848,71 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>2145</v>
+      <c r="A37" s="36">
+        <v>2044</v>
       </c>
       <c r="B37" s="2">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C37" s="2">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F37" s="2">
         <v>2</v>
       </c>
       <c r="G37" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H37" s="2">
         <v>0</v>
       </c>
       <c r="I37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="2">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="K37" s="2">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="L37" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M37" s="2">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>2160</v>
+      <c r="A38" s="36">
+        <v>2046</v>
       </c>
       <c r="B38" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C38" s="2">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>2</v>
+      </c>
+      <c r="G38" s="2">
         <v>3</v>
       </c>
-      <c r="D38" s="2">
-        <v>2</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0</v>
-      </c>
-      <c r="F38" s="2">
-        <v>8</v>
-      </c>
-      <c r="G38" s="2">
-        <v>9</v>
-      </c>
       <c r="H38" s="2">
         <v>0</v>
       </c>
@@ -14790,74 +14920,74 @@
         <v>1</v>
       </c>
       <c r="J38" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K38" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L38" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M38" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>2191</v>
+      <c r="A39" s="36">
+        <v>2145</v>
       </c>
       <c r="B39" s="2">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H39" s="2">
         <v>0</v>
       </c>
       <c r="I39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="2">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="K39" s="2">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="L39" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>2205</v>
+      <c r="A40" s="36">
+        <v>2160</v>
       </c>
       <c r="B40" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C40" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D40" s="2">
         <v>2</v>
@@ -14866,54 +14996,54 @@
         <v>0</v>
       </c>
       <c r="F40" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G40" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H40" s="2">
         <v>0</v>
       </c>
       <c r="I40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K40" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L40" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M40" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <v>2226</v>
+      <c r="A41" s="36">
+        <v>2191</v>
       </c>
       <c r="B41" s="2">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C41" s="2">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D41" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H41" s="2">
         <v>0</v>
@@ -14922,13 +15052,13 @@
         <v>0</v>
       </c>
       <c r="J41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="2">
         <v>0</v>
       </c>
       <c r="L41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M41" s="2">
         <v>0</v>
@@ -14938,26 +15068,26 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>2298</v>
+      <c r="A42" s="36">
+        <v>2205</v>
       </c>
       <c r="B42" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C42" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D42" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42" s="2">
         <v>0</v>
       </c>
       <c r="F42" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
@@ -14982,41 +15112,41 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
-        <v>2325</v>
+      <c r="A43" s="36">
+        <v>2226</v>
       </c>
       <c r="B43" s="2">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C43" s="2">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D43" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E43" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F43" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G43" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" s="2">
         <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
       </c>
       <c r="L43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="2">
         <v>0</v>
@@ -15026,14 +15156,14 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
-        <v>2329</v>
+      <c r="A44" s="36">
+        <v>2298</v>
       </c>
       <c r="B44" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C44" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D44" s="2">
         <v>0</v>
@@ -15042,10 +15172,10 @@
         <v>0</v>
       </c>
       <c r="F44" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G44" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H44" s="2">
         <v>0</v>
@@ -15054,13 +15184,13 @@
         <v>0</v>
       </c>
       <c r="J44" s="2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M44" s="2">
         <v>0</v>
@@ -15070,41 +15200,41 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
-        <v>2349</v>
+      <c r="A45" s="36">
+        <v>2325</v>
       </c>
       <c r="B45" s="2">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C45" s="2">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D45" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E45" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F45" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G45" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="2">
         <v>0</v>
       </c>
       <c r="J45" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="K45" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L45" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M45" s="2">
         <v>0</v>
@@ -15114,85 +15244,85 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>2397</v>
+      <c r="A46" s="36">
+        <v>2329</v>
       </c>
       <c r="B46" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C46" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E46" s="2">
         <v>0</v>
       </c>
       <c r="F46" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G46" s="2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
       </c>
       <c r="I46" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J46" s="2">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K46" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="L46" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M46" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
-        <v>2434</v>
+      <c r="A47" s="36">
+        <v>2349</v>
       </c>
       <c r="B47" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C47" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E47" s="2">
         <v>0</v>
       </c>
       <c r="F47" s="2">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="G47" s="2">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="H47" s="2">
         <v>0</v>
       </c>
       <c r="I47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" s="2">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="K47" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L47" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M47" s="2">
         <v>0</v>
@@ -15202,114 +15332,114 @@
       <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <v>2445</v>
+      <c r="A48" s="36">
+        <v>2397</v>
       </c>
       <c r="B48" s="2">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C48" s="2">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D48" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E48" s="2">
         <v>0</v>
       </c>
       <c r="F48" s="2">
+        <v>16</v>
+      </c>
+      <c r="G48" s="2">
+        <v>19</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
         <v>3</v>
       </c>
-      <c r="G48" s="2">
-        <v>3</v>
-      </c>
-      <c r="H48" s="2">
-        <v>0</v>
-      </c>
-      <c r="I48" s="2">
-        <v>0</v>
-      </c>
       <c r="J48" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="K48" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
-        <v>2461</v>
+      <c r="A49" s="36">
+        <v>2434</v>
       </c>
       <c r="B49" s="2">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C49" s="2">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D49" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E49" s="2">
         <v>0</v>
       </c>
       <c r="F49" s="2">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="G49" s="2">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="H49" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K49" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
-        <v>2487</v>
+      <c r="A50" s="36">
+        <v>2445</v>
       </c>
       <c r="B50" s="2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C50" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D50" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
       </c>
       <c r="F50" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G50" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H50" s="2">
         <v>0</v>
@@ -15318,13 +15448,13 @@
         <v>0</v>
       </c>
       <c r="J50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" s="2">
         <v>0</v>
       </c>
       <c r="L50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" s="2">
         <v>0</v>
@@ -15334,70 +15464,70 @@
       <c r="P50" s="2"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
-        <v>2493</v>
+      <c r="A51" s="36">
+        <v>2461</v>
       </c>
       <c r="B51" s="2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C51" s="2">
+        <v>16</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2">
+        <v>9</v>
+      </c>
+      <c r="G51" s="2">
+        <v>7</v>
+      </c>
+      <c r="H51" s="2">
+        <v>2</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2">
+        <v>7</v>
+      </c>
+      <c r="K51" s="2">
         <v>8</v>
       </c>
-      <c r="D51" s="2">
-        <v>3</v>
-      </c>
-      <c r="E51" s="2">
-        <v>0</v>
-      </c>
-      <c r="F51" s="2">
-        <v>0</v>
-      </c>
-      <c r="G51" s="2">
-        <v>0</v>
-      </c>
-      <c r="H51" s="2">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2">
-        <v>0</v>
-      </c>
-      <c r="J51" s="2">
-        <v>5</v>
-      </c>
-      <c r="K51" s="2">
-        <v>5</v>
-      </c>
       <c r="L51" s="2">
         <v>0</v>
       </c>
       <c r="M51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
-        <v>2494</v>
+      <c r="A52" s="36">
+        <v>2487</v>
       </c>
       <c r="B52" s="2">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="C52" s="2">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="D52" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E52" s="2">
         <v>0</v>
       </c>
       <c r="F52" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G52" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H52" s="2">
         <v>0</v>
@@ -15406,13 +15536,13 @@
         <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" s="2">
         <v>0</v>
       </c>
       <c r="L52" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52" s="2">
         <v>0</v>
@@ -15422,41 +15552,41 @@
       <c r="P52" s="2"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>2538</v>
+      <c r="A53" s="36">
+        <v>2493</v>
       </c>
       <c r="B53" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D53" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E53" s="2">
         <v>0</v>
       </c>
       <c r="F53" s="2">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G53" s="2">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="H53" s="2">
         <v>0</v>
       </c>
       <c r="I53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K53" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M53" s="2">
         <v>0</v>
@@ -15466,41 +15596,41 @@
       <c r="P53" s="2"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>2616</v>
+      <c r="A54" s="36">
+        <v>2494</v>
       </c>
       <c r="B54" s="2">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C54" s="2">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="D54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="2">
         <v>0</v>
       </c>
       <c r="F54" s="2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G54" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" s="2">
         <v>0</v>
       </c>
       <c r="J54" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K54" s="2">
         <v>0</v>
       </c>
       <c r="L54" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M54" s="2">
         <v>0</v>
@@ -15510,14 +15640,14 @@
       <c r="P54" s="2"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
-        <v>2735</v>
+      <c r="A55" s="36">
+        <v>2538</v>
       </c>
       <c r="B55" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C55" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D55" s="2">
         <v>0</v>
@@ -15526,25 +15656,25 @@
         <v>0</v>
       </c>
       <c r="F55" s="2">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="G55" s="2">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="H55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K55" s="2">
         <v>0</v>
       </c>
       <c r="L55" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M55" s="2">
         <v>0</v>
@@ -15554,8 +15684,8 @@
       <c r="P55" s="2"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
-        <v>2784</v>
+      <c r="A56" s="36">
+        <v>2616</v>
       </c>
       <c r="B56" s="2">
         <v>1</v>
@@ -15570,25 +15700,25 @@
         <v>0</v>
       </c>
       <c r="F56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" s="2">
         <v>0</v>
       </c>
       <c r="H56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="2">
         <v>0</v>
       </c>
       <c r="J56" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K56" s="2">
         <v>0</v>
       </c>
       <c r="L56" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M56" s="2">
         <v>0</v>
@@ -15598,29 +15728,29 @@
       <c r="P56" s="2"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
-        <v>2810</v>
+      <c r="A57" s="36">
+        <v>2735</v>
       </c>
       <c r="B57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
       </c>
       <c r="D57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" s="2">
         <v>0</v>
       </c>
       <c r="F57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="2">
         <v>0</v>
       </c>
       <c r="H57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="2">
         <v>0</v>
@@ -15642,8 +15772,8 @@
       <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
-        <v>2834</v>
+      <c r="A58" s="36">
+        <v>2784</v>
       </c>
       <c r="B58" s="2">
         <v>1</v>
@@ -15670,33 +15800,33 @@
         <v>0</v>
       </c>
       <c r="J58" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K58" s="2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L58" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M58" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
-        <v>2901</v>
+      <c r="A59" s="36">
+        <v>2810</v>
       </c>
       <c r="B59" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C59" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
@@ -15705,22 +15835,22 @@
         <v>0</v>
       </c>
       <c r="G59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" s="2">
         <v>0</v>
       </c>
       <c r="I59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K59" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L59" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M59" s="2">
         <v>0</v>
@@ -15730,61 +15860,61 @@
       <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>2942</v>
+      <c r="A60" s="36">
+        <v>2834</v>
       </c>
       <c r="B60" s="2">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="C60" s="2">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="D60" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F60" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G60" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H60" s="2">
         <v>0</v>
       </c>
       <c r="I60" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J60" s="2">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K60" s="2">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="L60" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M60" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="2">
-        <v>2985</v>
+      <c r="A61" s="36">
+        <v>2901</v>
       </c>
       <c r="B61" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C61" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D61" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E61" s="2">
         <v>0</v>
@@ -15793,22 +15923,22 @@
         <v>0</v>
       </c>
       <c r="G61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="2">
         <v>0</v>
       </c>
       <c r="I61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K61" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61" s="2">
         <v>0</v>
@@ -15818,82 +15948,170 @@
       <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
-        <v>3044</v>
+      <c r="A62" s="36">
+        <v>2942</v>
       </c>
       <c r="B62" s="2">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="C62" s="2">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D62" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E62" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G62" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J62" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K62" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L62" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M62" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
+      <c r="A63" s="36">
+        <v>2985</v>
+      </c>
+      <c r="B63" s="2">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2</v>
+      </c>
+      <c r="D63" s="2">
+        <v>2</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <v>0</v>
+      </c>
+      <c r="J63" s="2">
+        <v>0</v>
+      </c>
+      <c r="K63" s="2">
+        <v>0</v>
+      </c>
+      <c r="L63" s="2">
+        <v>0</v>
+      </c>
+      <c r="M63" s="2">
+        <v>0</v>
+      </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
+      <c r="A64" s="36">
+        <v>3044</v>
+      </c>
+      <c r="B64" s="2">
+        <v>4</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>4</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2">
+        <v>1</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2">
+        <v>0</v>
+      </c>
+      <c r="K64" s="2">
+        <v>0</v>
+      </c>
+      <c r="L64" s="2">
+        <v>0</v>
+      </c>
+      <c r="M64" s="2">
+        <v>0</v>
+      </c>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -15924,26 +16142,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
       <c r="N1" s="17" t="s">
         <v>23</v>
       </c>

</xml_diff>